<commit_message>
Opt with week and scenario runable
</commit_message>
<xml_diff>
--- a/input/input_big.xlsx
+++ b/input/input_big.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ESchr\workspace\uni\ATIS3\Single_Project\ATIES3_single_project_ES\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CB6263-068E-46F5-AC91-950C3B2268BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9998EA2F-EFFE-4455-9EB4-C254A5FF9972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="5" xr2:uid="{F41D6B2C-A29F-4016-AF80-C7BE5C33C0CD}"/>
+    <workbookView xWindow="345" yWindow="9015" windowWidth="7635" windowHeight="4650" xr2:uid="{F41D6B2C-A29F-4016-AF80-C7BE5C33C0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="bilateral_contract_data" sheetId="1" r:id="rId1"/>
@@ -784,12 +784,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326D2C6A-7C1E-476A-9A89-D087E262AE4F}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -885,7 +887,7 @@
         <v>25</v>
       </c>
       <c r="B4">
-        <v>55.4</v>
+        <v>48.5</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -914,7 +916,7 @@
         <v>26</v>
       </c>
       <c r="B5">
-        <v>64.099999999999994</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -943,7 +945,7 @@
         <v>27</v>
       </c>
       <c r="B6">
-        <v>45.9</v>
+        <v>49.5</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -972,7 +974,7 @@
         <v>28</v>
       </c>
       <c r="B7">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C7">
         <v>40</v>
@@ -1001,7 +1003,7 @@
         <v>118</v>
       </c>
       <c r="B8">
-        <v>56.7</v>
+        <v>49</v>
       </c>
       <c r="C8">
         <v>50</v>
@@ -1030,7 +1032,7 @@
         <v>119</v>
       </c>
       <c r="B9">
-        <v>63.2</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>40</v>
@@ -1180,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE0D819-36A6-4670-8860-D1C2902FF7CD}">
   <dimension ref="A1:CG2"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,100 +1462,100 @@
         <v>275</v>
       </c>
       <c r="F2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G2">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="H2">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="I2">
-        <v>250.42857142857099</v>
+        <v>275</v>
       </c>
       <c r="J2">
-        <v>254.5</v>
+        <v>200</v>
       </c>
       <c r="K2">
-        <v>258.57142857142901</v>
+        <v>250</v>
       </c>
       <c r="L2">
-        <v>262.642857142857</v>
+        <v>225</v>
       </c>
       <c r="M2">
-        <v>266.71428571428601</v>
+        <v>275</v>
       </c>
       <c r="N2">
-        <v>270.78571428571399</v>
+        <v>200</v>
       </c>
       <c r="O2">
+        <v>250</v>
+      </c>
+      <c r="P2">
+        <v>225</v>
+      </c>
+      <c r="Q2">
+        <v>275</v>
+      </c>
+      <c r="R2">
         <v>200</v>
       </c>
-      <c r="P2">
+      <c r="S2">
         <v>250</v>
       </c>
-      <c r="Q2">
+      <c r="T2">
         <v>225</v>
       </c>
-      <c r="R2">
+      <c r="U2">
         <v>275</v>
       </c>
-      <c r="S2">
-        <v>199</v>
-      </c>
-      <c r="T2">
-        <v>230</v>
-      </c>
-      <c r="U2">
-        <v>260</v>
-      </c>
       <c r="V2">
-        <v>250.42857142857099</v>
+        <v>200</v>
       </c>
       <c r="W2">
-        <v>254.5</v>
+        <v>250</v>
       </c>
       <c r="X2">
-        <v>258.57142857142901</v>
+        <v>225</v>
       </c>
       <c r="Y2">
-        <v>262.642857142857</v>
+        <v>275</v>
       </c>
       <c r="Z2">
-        <v>266.71428571428601</v>
+        <v>200</v>
       </c>
       <c r="AA2">
-        <v>257.02428571428601</v>
+        <v>250</v>
       </c>
       <c r="AB2">
-        <v>257.92</v>
+        <v>225</v>
       </c>
       <c r="AC2">
-        <v>258.81571428571402</v>
+        <v>275</v>
       </c>
       <c r="AD2">
-        <v>259.711428571429</v>
+        <v>200</v>
       </c>
       <c r="AE2">
-        <v>260.607142857143</v>
+        <v>250</v>
       </c>
       <c r="AF2">
-        <v>261.50285714285701</v>
+        <v>225</v>
       </c>
       <c r="AG2">
-        <v>262.39857142857102</v>
+        <v>275</v>
       </c>
       <c r="AH2">
-        <v>263.29428571428599</v>
+        <v>200</v>
       </c>
       <c r="AI2">
-        <v>264.19</v>
+        <v>250</v>
       </c>
       <c r="AJ2">
-        <v>265.085714285714</v>
+        <v>225</v>
       </c>
       <c r="AK2">
-        <v>265.98142857142898</v>
+        <v>275</v>
       </c>
       <c r="AL2">
         <v>200</v>
@@ -1568,136 +1570,136 @@
         <v>275</v>
       </c>
       <c r="AP2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AQ2">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="AR2">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="AS2">
-        <v>250.42857142857099</v>
+        <v>275</v>
       </c>
       <c r="AT2">
-        <v>254.5</v>
+        <v>200</v>
       </c>
       <c r="AU2">
-        <v>258.57142857142901</v>
+        <v>250</v>
       </c>
       <c r="AV2">
-        <v>262.642857142857</v>
+        <v>225</v>
       </c>
       <c r="AW2">
-        <v>266.71428571428601</v>
+        <v>275</v>
       </c>
       <c r="AX2">
-        <v>270.78571428571399</v>
+        <v>200</v>
       </c>
       <c r="AY2">
+        <v>250</v>
+      </c>
+      <c r="AZ2">
+        <v>225</v>
+      </c>
+      <c r="BA2">
+        <v>275</v>
+      </c>
+      <c r="BB2">
         <v>200</v>
       </c>
-      <c r="AZ2">
+      <c r="BC2">
         <v>250</v>
       </c>
-      <c r="BA2">
+      <c r="BD2">
         <v>225</v>
       </c>
-      <c r="BB2">
+      <c r="BE2">
         <v>275</v>
       </c>
-      <c r="BC2">
-        <v>199</v>
-      </c>
-      <c r="BD2">
-        <v>230</v>
-      </c>
-      <c r="BE2">
-        <v>260</v>
-      </c>
       <c r="BF2">
-        <v>250.42857142857099</v>
+        <v>200</v>
       </c>
       <c r="BG2">
-        <v>254.5</v>
+        <v>250</v>
       </c>
       <c r="BH2">
-        <v>258.57142857142901</v>
+        <v>225</v>
       </c>
       <c r="BI2">
-        <v>262.642857142857</v>
+        <v>275</v>
       </c>
       <c r="BJ2">
-        <v>251.14192251815999</v>
+        <v>200</v>
       </c>
       <c r="BK2">
-        <v>251.245582741238</v>
+        <v>250</v>
       </c>
       <c r="BL2">
-        <v>251.34924296431601</v>
+        <v>225</v>
       </c>
       <c r="BM2">
-        <v>251.45290318739299</v>
+        <v>275</v>
       </c>
       <c r="BN2">
-        <v>251.556563410471</v>
+        <v>200</v>
       </c>
       <c r="BO2">
-        <v>251.66022363354901</v>
+        <v>250</v>
       </c>
       <c r="BP2">
-        <v>251.76388385662699</v>
+        <v>225</v>
       </c>
       <c r="BQ2">
-        <v>251.867544079705</v>
+        <v>275</v>
       </c>
       <c r="BR2">
-        <v>251.97120430278301</v>
+        <v>200</v>
       </c>
       <c r="BS2">
-        <v>252.07486452585999</v>
+        <v>250</v>
       </c>
       <c r="BT2">
-        <v>252.178524748938</v>
+        <v>225</v>
       </c>
       <c r="BU2">
-        <v>252.28218497201601</v>
+        <v>275</v>
       </c>
       <c r="BV2">
-        <v>252.38584519509399</v>
+        <v>200</v>
       </c>
       <c r="BW2">
-        <v>252.489505418172</v>
+        <v>250</v>
       </c>
       <c r="BX2">
-        <v>252.59316564125001</v>
+        <v>225</v>
       </c>
       <c r="BY2">
-        <v>252.696825864327</v>
+        <v>275</v>
       </c>
       <c r="BZ2">
-        <v>252.80048608740501</v>
+        <v>200</v>
       </c>
       <c r="CA2">
-        <v>252.90414631048299</v>
+        <v>250</v>
       </c>
       <c r="CB2">
-        <v>253.00780653356099</v>
+        <v>225</v>
       </c>
       <c r="CC2">
-        <v>253.111466756639</v>
+        <v>275</v>
       </c>
       <c r="CD2">
-        <v>253.21512697971701</v>
+        <v>200</v>
       </c>
       <c r="CE2">
-        <v>253.318787202794</v>
+        <v>250</v>
       </c>
       <c r="CF2">
-        <v>253.42244742587201</v>
+        <v>225</v>
       </c>
       <c r="CG2">
-        <v>253.52610764894999</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -6095,7 +6097,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6382,7 +6384,7 @@
   <dimension ref="A1:CG16"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="CG2" sqref="CG2:CG16"/>
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8517,7 +8519,7 @@
         <v>0</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -10512,7 +10514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4D9919-2431-4026-8FD6-F5920B77E3EE}">
   <dimension ref="A1:CG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Spring price scenarios generated
</commit_message>
<xml_diff>
--- a/input/input_big.xlsx
+++ b/input/input_big.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ESchr\workspace\uni\ATIS3\Single_Project\ATIES3_single_project_ES\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9998EA2F-EFFE-4455-9EB4-C254A5FF9972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D584887A-112C-4A53-9E41-6FE119AA8240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="9015" windowWidth="7635" windowHeight="4650" xr2:uid="{F41D6B2C-A29F-4016-AF80-C7BE5C33C0CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{F41D6B2C-A29F-4016-AF80-C7BE5C33C0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="bilateral_contract_data" sheetId="1" r:id="rId1"/>
@@ -784,7 +784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326D2C6A-7C1E-476A-9A89-D087E262AE4F}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1711,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD436EB6-D80F-424D-BA0F-03D2C90350F3}">
   <dimension ref="A1:CG17"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="BM1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="CC19" sqref="CC19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,61 +1982,61 @@
         <v>44</v>
       </c>
       <c r="C2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F2">
         <v>44</v>
       </c>
       <c r="G2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J2">
         <v>44</v>
       </c>
       <c r="K2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N2">
         <v>44</v>
       </c>
       <c r="O2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R2">
         <v>44</v>
       </c>
       <c r="S2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V2">
         <v>44</v>
@@ -2239,61 +2239,61 @@
         <v>44</v>
       </c>
       <c r="C3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E3">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F3">
         <v>44</v>
       </c>
       <c r="G3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I3">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J3">
         <v>44</v>
       </c>
       <c r="K3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M3">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N3">
         <v>44</v>
       </c>
       <c r="O3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q3">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R3">
         <v>44</v>
       </c>
       <c r="S3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U3">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V3">
         <v>44</v>
@@ -2496,61 +2496,61 @@
         <v>44</v>
       </c>
       <c r="C4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E4">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F4">
         <v>44</v>
       </c>
       <c r="G4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I4">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J4">
         <v>44</v>
       </c>
       <c r="K4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M4">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N4">
         <v>44</v>
       </c>
       <c r="O4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q4">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R4">
         <v>44</v>
       </c>
       <c r="S4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U4">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V4">
         <v>44</v>
@@ -2753,61 +2753,61 @@
         <v>44</v>
       </c>
       <c r="C5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E5">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F5">
         <v>44</v>
       </c>
       <c r="G5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I5">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J5">
         <v>44</v>
       </c>
       <c r="K5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M5">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N5">
         <v>44</v>
       </c>
       <c r="O5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q5">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R5">
         <v>44</v>
       </c>
       <c r="S5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U5">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V5">
         <v>44</v>
@@ -3010,61 +3010,61 @@
         <v>44</v>
       </c>
       <c r="C6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F6">
         <v>44</v>
       </c>
       <c r="G6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H6">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J6">
         <v>44</v>
       </c>
       <c r="K6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N6">
         <v>44</v>
       </c>
       <c r="O6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P6">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R6">
         <v>44</v>
       </c>
       <c r="S6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T6">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U6">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V6">
         <v>44</v>
@@ -3267,61 +3267,61 @@
         <v>44</v>
       </c>
       <c r="C7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F7">
         <v>44</v>
       </c>
       <c r="G7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J7">
         <v>44</v>
       </c>
       <c r="K7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N7">
         <v>44</v>
       </c>
       <c r="O7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P7">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R7">
         <v>44</v>
       </c>
       <c r="S7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T7">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V7">
         <v>44</v>
@@ -3524,61 +3524,61 @@
         <v>44</v>
       </c>
       <c r="C8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E8">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F8">
         <v>44</v>
       </c>
       <c r="G8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I8">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J8">
         <v>44</v>
       </c>
       <c r="K8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L8">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M8">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N8">
         <v>44</v>
       </c>
       <c r="O8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P8">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q8">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R8">
         <v>44</v>
       </c>
       <c r="S8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T8">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U8">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V8">
         <v>44</v>
@@ -3781,61 +3781,61 @@
         <v>44</v>
       </c>
       <c r="C9">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F9">
         <v>44</v>
       </c>
       <c r="G9">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I9">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J9">
         <v>44</v>
       </c>
       <c r="K9">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L9">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M9">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N9">
         <v>44</v>
       </c>
       <c r="O9">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P9">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q9">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R9">
         <v>44</v>
       </c>
       <c r="S9">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T9">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U9">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V9">
         <v>44</v>
@@ -4038,61 +4038,61 @@
         <v>50</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F10">
         <v>50</v>
       </c>
       <c r="G10">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J10">
         <v>50</v>
       </c>
       <c r="K10">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N10">
         <v>50</v>
       </c>
       <c r="O10">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R10">
         <v>50</v>
       </c>
       <c r="S10">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V10">
         <v>50</v>
@@ -4295,61 +4295,61 @@
         <v>50</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E11">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F11">
         <v>50</v>
       </c>
       <c r="G11">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H11">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I11">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J11">
         <v>50</v>
       </c>
       <c r="K11">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L11">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M11">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N11">
         <v>50</v>
       </c>
       <c r="O11">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P11">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q11">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R11">
         <v>50</v>
       </c>
       <c r="S11">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T11">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U11">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V11">
         <v>50</v>
@@ -4552,61 +4552,61 @@
         <v>50</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F12">
         <v>50</v>
       </c>
       <c r="G12">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J12">
         <v>50</v>
       </c>
       <c r="K12">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N12">
         <v>50</v>
       </c>
       <c r="O12">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R12">
         <v>50</v>
       </c>
       <c r="S12">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V12">
         <v>50</v>
@@ -4809,61 +4809,61 @@
         <v>50</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F13">
         <v>50</v>
       </c>
       <c r="G13">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J13">
         <v>50</v>
       </c>
       <c r="K13">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N13">
         <v>50</v>
       </c>
       <c r="O13">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R13">
         <v>50</v>
       </c>
       <c r="S13">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V13">
         <v>50</v>
@@ -5066,61 +5066,61 @@
         <v>50</v>
       </c>
       <c r="C14">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F14">
         <v>50</v>
       </c>
       <c r="G14">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J14">
         <v>50</v>
       </c>
       <c r="K14">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N14">
         <v>50</v>
       </c>
       <c r="O14">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R14">
         <v>50</v>
       </c>
       <c r="S14">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V14">
         <v>50</v>
@@ -5323,61 +5323,61 @@
         <v>50</v>
       </c>
       <c r="C15">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F15">
         <v>50</v>
       </c>
       <c r="G15">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J15">
         <v>50</v>
       </c>
       <c r="K15">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N15">
         <v>50</v>
       </c>
       <c r="O15">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R15">
         <v>50</v>
       </c>
       <c r="S15">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V15">
         <v>50</v>
@@ -5580,61 +5580,61 @@
         <v>50</v>
       </c>
       <c r="C16">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F16">
         <v>50</v>
       </c>
       <c r="G16">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J16">
         <v>50</v>
       </c>
       <c r="K16">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N16">
         <v>50</v>
       </c>
       <c r="O16">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R16">
         <v>50</v>
       </c>
       <c r="S16">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V16">
         <v>50</v>
@@ -5837,61 +5837,61 @@
         <v>50</v>
       </c>
       <c r="C17">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E17">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F17">
         <v>50</v>
       </c>
       <c r="G17">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H17">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I17">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J17">
         <v>50</v>
       </c>
       <c r="K17">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L17">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M17">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N17">
         <v>50</v>
       </c>
       <c r="O17">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P17">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q17">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R17">
         <v>50</v>
       </c>
       <c r="S17">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T17">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U17">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V17">
         <v>50</v>
@@ -6026,61 +6026,61 @@
         <v>53</v>
       </c>
       <c r="BN17">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BO17">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="BP17">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="BQ17">
         <v>53</v>
       </c>
       <c r="BR17">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BS17">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="BT17">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="BU17">
         <v>53</v>
       </c>
       <c r="BV17">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BW17">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="BX17">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="BY17">
         <v>53</v>
       </c>
       <c r="BZ17">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="CA17">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="CB17">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="CC17">
         <v>53</v>
       </c>
       <c r="CD17">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="CE17">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="CF17">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="CG17">
         <v>53</v>

</xml_diff>